<commit_message>
Update Ada code to work with moving digital pins from pio package to the more general GPIO. Update Pinout.xlsx to properly identify pin 1 and to note that pin 4 is driven by both PA29 and PC26.
</commit_message>
<xml_diff>
--- a/Pinout.xlsx
+++ b/Pinout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="623">
   <si>
     <t xml:space="preserve">Table 1</t>
   </si>
@@ -1881,6 +1881,15 @@
   </si>
   <si>
     <t xml:space="preserve">Slow clock oscillator output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/TX0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD-CS, wired to PC26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wired to PA29</t>
   </si>
 </sst>
 </file>
@@ -2040,12 +2049,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.9"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="17.234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.6428571428572"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="17.234693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="20.5102040816327"/>
-    <col collapsed="false" hidden="false" max="256" min="11" style="1" width="17.234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="17.234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="45.0408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="19"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="22.6530612244898"/>
+    <col collapsed="false" hidden="false" max="256" min="11" style="1" width="19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5762,17 +5770,16 @@
   <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.9"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="17.234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="1" width="20.5102040816327"/>
-    <col collapsed="false" hidden="false" max="251" min="6" style="1" width="17.234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="17.234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="1" width="22.6530612244898"/>
+    <col collapsed="false" hidden="false" max="251" min="6" style="1" width="19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5794,1146 +5801,1146 @@
     </row>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>350</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>354</v>
+        <v>16</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>355</v>
+        <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="E2" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>357</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>361</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>362</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="E3" s="6"/>
+        <v>620</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>372</v>
+        <v>26</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>376</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>377</v>
+        <v>31</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="E4" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>378</v>
+        <v>34</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>382</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>383</v>
+        <v>31</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="E5" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>384</v>
+        <v>40</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>388</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>389</v>
+        <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>298</v>
+        <v>46</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>390</v>
+        <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>394</v>
+        <v>50</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>395</v>
+        <v>51</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>237</v>
+        <v>52</v>
       </c>
       <c r="E7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>396</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>400</v>
+        <v>57</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>401</v>
+        <v>58</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>59</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>403</v>
+        <v>61</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>407</v>
+        <v>64</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>408</v>
+        <v>65</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>170</v>
+        <v>66</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>409</v>
+        <v>67</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>411</v>
+        <v>69</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>412</v>
+        <v>70</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>413</v>
+        <v>72</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>416</v>
+        <v>75</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>417</v>
+        <v>76</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>418</v>
+        <v>77</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>363</v>
+        <v>78</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>366</v>
+        <v>79</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>367</v>
+        <v>81</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="E12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>368</v>
+        <v>83</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>370</v>
+        <v>84</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>371</v>
+        <v>86</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>146</v>
+        <v>87</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>315</v>
+        <v>88</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>318</v>
+        <v>91</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>319</v>
+        <v>92</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>320</v>
+        <v>93</v>
       </c>
       <c r="E14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="E15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>419</v>
+        <v>100</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>420</v>
+        <v>103</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>423</v>
+        <v>104</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>424</v>
+        <v>105</v>
       </c>
       <c r="E16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>425</v>
+        <v>106</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>426</v>
+        <v>109</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>427</v>
+        <v>110</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>428</v>
+        <v>111</v>
       </c>
       <c r="E17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>321</v>
+        <v>112</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>323</v>
+        <v>116</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>324</v>
+        <v>117</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>325</v>
+        <v>118</v>
       </c>
       <c r="E18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>429</v>
+        <v>119</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>432</v>
+        <v>123</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>433</v>
+        <v>124</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>434</v>
+        <v>125</v>
       </c>
       <c r="E19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>435</v>
+        <v>126</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>437</v>
+        <v>129</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>438</v>
+        <v>130</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>437</v>
+        <v>131</v>
       </c>
       <c r="E20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="E21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="E22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="E23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="E24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="E25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="E26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="E27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="E28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="E30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="E32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="E33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="E34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="E36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="E37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="E38" s="6"/>
+        <v>234</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="E39" s="6"/>
+        <v>239</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="E42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="E43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="E45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="E46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="E47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="E49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="E50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
-        <v>100</v>
+        <v>303</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>103</v>
+        <v>306</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>104</v>
+        <v>307</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>105</v>
+        <v>308</v>
       </c>
       <c r="E51" s="6"/>
     </row>
     <row r="52" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>169</v>
+        <v>309</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>172</v>
+        <v>312</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>173</v>
+        <v>313</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>174</v>
+        <v>314</v>
       </c>
       <c r="E52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="E53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="E54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="E55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>40</v>
+        <v>344</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>44</v>
+        <v>347</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>45</v>
+        <v>348</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>46</v>
+        <v>349</v>
       </c>
       <c r="E58" s="6"/>
     </row>
     <row r="59" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>47</v>
+        <v>350</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>50</v>
+        <v>354</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>51</v>
+        <v>355</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>52</v>
+        <v>356</v>
       </c>
       <c r="E59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>53</v>
+        <v>357</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>57</v>
+        <v>361</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>58</v>
+        <v>362</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="E60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>11</v>
+        <v>363</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>16</v>
+        <v>366</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>17</v>
+        <v>367</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="E61" s="6"/>
     </row>
     <row r="62" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
-        <v>72</v>
+        <v>368</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>75</v>
+        <v>370</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>76</v>
+        <v>371</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
       <c r="E62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
-        <v>83</v>
+        <v>372</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>84</v>
+        <v>376</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>86</v>
+        <v>377</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>87</v>
+        <v>333</v>
       </c>
       <c r="E63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
-        <v>94</v>
+        <v>378</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>97</v>
+        <v>382</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>98</v>
+        <v>383</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>99</v>
+        <v>327</v>
       </c>
       <c r="E64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
-        <v>112</v>
+        <v>384</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>116</v>
+        <v>388</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>117</v>
+        <v>389</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>118</v>
+        <v>298</v>
       </c>
       <c r="E65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
-        <v>451</v>
+        <v>390</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>455</v>
+        <v>394</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>456</v>
+        <v>395</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>455</v>
+        <v>237</v>
       </c>
       <c r="E66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
-        <v>106</v>
+        <v>396</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>109</v>
+        <v>400</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>110</v>
+        <v>401</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>111</v>
+        <v>402</v>
       </c>
       <c r="E67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
-        <v>457</v>
+        <v>403</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>460</v>
+        <v>407</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>461</v>
+        <v>408</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>460</v>
+        <v>170</v>
       </c>
       <c r="E68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
-        <v>26</v>
+        <v>409</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>30</v>
+        <v>411</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>31</v>
+        <v>412</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
-        <v>34</v>
+        <v>413</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>30</v>
+        <v>416</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>31</v>
+        <v>417</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>39</v>
-      </c>
+        <v>418</v>
+      </c>
+      <c r="E70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
-        <v>229</v>
+        <v>419</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>232</v>
+        <v>420</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>233</v>
+        <v>423</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>235</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="E71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>236</v>
+        <v>425</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>232</v>
+        <v>426</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>233</v>
+        <v>427</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>39</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="E72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
-        <v>20</v>
+        <v>429</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>23</v>
+        <v>432</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>24</v>
+        <v>433</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="E73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
-        <v>61</v>
+        <v>435</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>64</v>
+        <v>437</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>65</v>
+        <v>438</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>66</v>
+        <v>437</v>
       </c>
       <c r="E74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
-        <v>78</v>
+        <v>439</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>81</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="C75" s="6"/>
       <c r="D75" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E75" s="6"/>
+        <v>442</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
-        <v>88</v>
+        <v>444</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>92</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="C76" s="6"/>
       <c r="D76" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E76" s="6"/>
+        <v>442</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>441</v>
@@ -6948,7 +6955,7 @@
     </row>
     <row r="78" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="5" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>441</v>
@@ -6963,33 +6970,33 @@
     </row>
     <row r="79" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="C79" s="6"/>
+        <v>455</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>456</v>
+      </c>
       <c r="D79" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>443</v>
-      </c>
+        <v>455</v>
+      </c>
+      <c r="E79" s="6"/>
     </row>
     <row r="80" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="C80" s="6"/>
+        <v>460</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>461</v>
+      </c>
       <c r="D80" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>446</v>
-      </c>
+        <v>460</v>
+      </c>
+      <c r="E80" s="6"/>
     </row>
     <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>